<commit_message>
test solution to #226
</commit_message>
<xml_diff>
--- a/run/output/iecorrect/iecorrect-missingid.xlsx
+++ b/run/output/iecorrect/iecorrect-missingid.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wb501238\Documents\GitHub\iefieldkit\run\output\iecorrect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B952038A-9195-49F9-BF96-CCFBE4975057}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F8B166C-22D6-4B59-85DE-CC3DA562EE6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="string" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
   <si>
     <t>make</t>
   </si>
@@ -464,7 +464,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -539,7 +539,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -580,7 +580,9 @@
       <c r="D2" s="1">
         <v>2</v>
       </c>
-      <c r="E2" s="1"/>
+      <c r="E2" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
@@ -593,7 +595,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>

</xml_diff>